<commit_message>
Continued: combinations from itertools
</commit_message>
<xml_diff>
--- a/bssids.xlsx
+++ b/bssids.xlsx
@@ -1769,7 +1769,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1794,7 +1794,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="6"/>
-      <c r="G1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>